<commit_message>
Added test data to be fetched from excel-sheet for Wishlist test
</commit_message>
<xml_diff>
--- a/src/test/java/Centric/ShoppingStoreTestData/excelData.xlsx
+++ b/src/test/java/Centric/ShoppingStoreTestData/excelData.xlsx
@@ -3,41 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sushant.bhatnagar\eclipse-workspace\ShoppingStore\src\test\java\Centric\ShoppingStoreTestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF747E-CF98-4CB8-A5EF-68B636757599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{51411BEF-53EE-4BE4-BFD8-A107D7F31DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1D45179B-BEF3-4E2D-8204-F79838531864}"/>
+    <workbookView xWindow="13245" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1D45179B-BEF3-4E2D-8204-F79838531864}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="PurchaseOrder" sheetId="2" r:id="rId2"/>
+    <sheet name="Wishlist" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:X13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>TestCases</t>
   </si>
@@ -70,6 +56,15 @@
   </si>
   <si>
     <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>HTC One M8 Android L 5.0 Lollipop</t>
+  </si>
+  <si>
+    <t>HTCWishList</t>
   </si>
 </sst>
 </file>
@@ -434,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D6B247-E8CD-46FD-A4E3-6252D818C22E}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,7 +487,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,4 +512,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F65A92-E3E1-4456-8CCD-F5AA7C4C9367}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>